<commit_message>
Uploading SQL Case homework, including bonus.  Still have yet to design ERD using quickdatabase diagram, to export an image of the diagram, and to generate a SQL file of the resulting table schemata.
</commit_message>
<xml_diff>
--- a/Case homework/EmployeeSQL/ERD_metadata.xlsx
+++ b/Case homework/EmployeeSQL/ERD_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brook\sql-challenge\Case homework\EmployeeSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365F9C99-B82E-4453-A1CF-15612FB65ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8EC53E-8162-49D2-A7EB-B417DB08A914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BA3A216-BB13-4DB0-9B4C-BACDC0A15B8B}"/>
   </bookViews>
@@ -137,7 +137,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +167,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,11 +261,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -567,10 +581,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37282600-14C9-4670-B217-54704465065F}">
-  <dimension ref="A1:N30"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L30" sqref="A1:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,27 +599,27 @@
     <col min="5" max="6" width="12.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="13" width="32.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="9" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="32.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="M1" s="1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -612,11 +629,11 @@
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>9</v>
       </c>
@@ -627,7 +644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
         <v>21</v>
@@ -640,38 +657,38 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="M4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="11">
+      <c r="L4" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="M6" s="11" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="K6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -681,14 +698,14 @@
       <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="3">
+      <c r="L7" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>331603</v>
       </c>
@@ -698,14 +715,14 @@
       <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="L8" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="9" t="s">
         <v>25</v>
@@ -719,31 +736,31 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="M10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="M11" s="8" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="K11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N11" s="3">
+      <c r="L11" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -753,11 +770,11 @@
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>24</v>
       </c>
@@ -768,7 +785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="9" t="s">
         <v>21</v>
@@ -782,20 +799,20 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -875,21 +892,21 @@
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -931,16 +948,16 @@
       <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -980,11 +997,12 @@
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="82" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>